<commit_message>
Fnnish basic sell and buy for top 50
</commit_message>
<xml_diff>
--- a/WhaleWatching/holders.xlsx
+++ b/WhaleWatching/holders.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,13 +25,21 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D8D8D9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -52,7 +60,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -61,7 +69,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -429,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,7 +503,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>760,657,099,923,234</t>
+          <t>760,733,598,377,011</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -503,16 +516,8 @@
           <t xml:space="preserve">0.7607% </t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>761 Trillion</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>760,657,099,923,234</t>
-        </is>
-      </c>
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -525,7 +530,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>755,756,548,665,561</t>
+          <t>755,805,960,029,718</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -538,16 +543,8 @@
           <t xml:space="preserve">0.7558% </t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>756 Trillion</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>755,756,548,665,561</t>
-        </is>
-      </c>
+      <c r="F3" s="2" t="n"/>
+      <c r="G3" s="2" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -560,7 +557,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>603,650,071,839,525</t>
+          <t>603,712,409,699,892</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -573,16 +570,8 @@
           <t xml:space="preserve">0.6037% </t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>604 Trillion</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
-        <is>
-          <t>603,650,071,839,525</t>
-        </is>
-      </c>
+      <c r="F4" s="2" t="n"/>
+      <c r="G4" s="2" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -595,12 +584,12 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>602,491,726,950,986</t>
+          <t>602,530,791,527,282</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>602 Trillion</t>
+          <t>603 Trillion</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
@@ -608,16 +597,8 @@
           <t xml:space="preserve">0.6025% </t>
         </is>
       </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>602 Trillion</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr">
-        <is>
-          <t>602,491,726,950,986</t>
-        </is>
-      </c>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="2" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -630,7 +611,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>549,662,717,019,826</t>
+          <t>549,698,341,865,050</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -643,16 +624,8 @@
           <t xml:space="preserve">0.5497% </t>
         </is>
       </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>550 Trillion</t>
-        </is>
-      </c>
-      <c r="G6" s="3" t="inlineStr">
-        <is>
-          <t>549,662,717,019,826</t>
-        </is>
-      </c>
+      <c r="F6" s="2" t="n"/>
+      <c r="G6" s="2" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -665,7 +638,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>524,112,586,891,433</t>
+          <t>524,146,288,497,680</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
@@ -678,16 +651,8 @@
           <t xml:space="preserve">0.5241% </t>
         </is>
       </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>524 Trillion</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="inlineStr">
-        <is>
-          <t>524,112,586,891,433</t>
-        </is>
-      </c>
+      <c r="F7" s="2" t="n"/>
+      <c r="G7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -700,7 +665,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>500,295,115,478,046</t>
+          <t>500,342,304,983,551</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
@@ -713,16 +678,8 @@
           <t xml:space="preserve">0.5003% </t>
         </is>
       </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>500 Trillion</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
-        <is>
-          <t>500,295,115,478,046</t>
-        </is>
-      </c>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -735,7 +692,7 @@
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>432,400,582,170,267</t>
+          <t>432,439,854,928,747</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
@@ -748,16 +705,8 @@
           <t xml:space="preserve">0.4324% </t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>432 Trillion</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="inlineStr">
-        <is>
-          <t>432,400,582,170,267</t>
-        </is>
-      </c>
+      <c r="F9" s="2" t="n"/>
+      <c r="G9" s="2" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -783,16 +732,8 @@
           <t xml:space="preserve">0.4200% </t>
         </is>
       </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>420 Trillion</t>
-        </is>
-      </c>
-      <c r="G10" s="3" t="inlineStr">
-        <is>
-          <t>419,994,932,243,674</t>
-        </is>
-      </c>
+      <c r="F10" s="2" t="n"/>
+      <c r="G10" s="2" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -805,7 +746,7 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>419,265,552,070,497</t>
+          <t>419,360,533,364,969</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
@@ -815,19 +756,11 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4193% </t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>419 Trillion</t>
-        </is>
-      </c>
-      <c r="G11" s="3" t="inlineStr">
-        <is>
-          <t>419,265,552,070,497</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.4194% </t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n"/>
+      <c r="G11" s="2" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -840,7 +773,7 @@
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>415,188,049,125,007</t>
+          <t>415,228,348,905,327</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
@@ -853,16 +786,8 @@
           <t xml:space="preserve">0.4152% </t>
         </is>
       </c>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>415 Trillion</t>
-        </is>
-      </c>
-      <c r="G12" s="3" t="inlineStr">
-        <is>
-          <t>415,188,049,125,007</t>
-        </is>
-      </c>
+      <c r="F12" s="2" t="n"/>
+      <c r="G12" s="2" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -888,16 +813,8 @@
           <t xml:space="preserve">0.4067% </t>
         </is>
       </c>
-      <c r="F13" s="2" t="inlineStr">
-        <is>
-          <t>407 Trillion</t>
-        </is>
-      </c>
-      <c r="G13" s="3" t="inlineStr">
-        <is>
-          <t>406,746,124,267,053</t>
-        </is>
-      </c>
+      <c r="F13" s="2" t="n"/>
+      <c r="G13" s="2" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -923,16 +840,8 @@
           <t xml:space="preserve">0.4060% </t>
         </is>
       </c>
-      <c r="F14" s="2" t="inlineStr">
-        <is>
-          <t>406 Trillion</t>
-        </is>
-      </c>
-      <c r="G14" s="3" t="inlineStr">
-        <is>
-          <t>405,964,100,208,639</t>
-        </is>
-      </c>
+      <c r="F14" s="2" t="n"/>
+      <c r="G14" s="2" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -945,12 +854,12 @@
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>362,477,591,762,882</t>
+          <t>362,521,477,411,729</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>362 Trillion</t>
+          <t>363 Trillion</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
@@ -958,16 +867,8 @@
           <t xml:space="preserve">0.3625% </t>
         </is>
       </c>
-      <c r="F15" s="2" t="inlineStr">
-        <is>
-          <t>362 Trillion</t>
-        </is>
-      </c>
-      <c r="G15" s="3" t="inlineStr">
-        <is>
-          <t>362,477,591,762,882</t>
-        </is>
-      </c>
+      <c r="F15" s="2" t="n"/>
+      <c r="G15" s="2" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -993,16 +894,8 @@
           <t xml:space="preserve">0.2632% </t>
         </is>
       </c>
-      <c r="F16" s="2" t="inlineStr">
-        <is>
-          <t>263 Trillion</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>263,241,099,413,936</t>
-        </is>
-      </c>
+      <c r="F16" s="2" t="n"/>
+      <c r="G16" s="2" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -1028,16 +921,8 @@
           <t xml:space="preserve">0.2500% </t>
         </is>
       </c>
-      <c r="F17" s="2" t="inlineStr">
-        <is>
-          <t>250 Trillion</t>
-        </is>
-      </c>
-      <c r="G17" s="3" t="inlineStr">
-        <is>
-          <t>250,044,900,251,963</t>
-        </is>
-      </c>
+      <c r="F17" s="2" t="n"/>
+      <c r="G17" s="2" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -1063,16 +948,8 @@
           <t xml:space="preserve">0.2174% </t>
         </is>
       </c>
-      <c r="F18" s="2" t="inlineStr">
-        <is>
-          <t>217 Trillion</t>
-        </is>
-      </c>
-      <c r="G18" s="3" t="inlineStr">
-        <is>
-          <t>217,372,420,035,141</t>
-        </is>
-      </c>
+      <c r="F18" s="2" t="n"/>
+      <c r="G18" s="2" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -1098,16 +975,8 @@
           <t xml:space="preserve">0.2067% </t>
         </is>
       </c>
-      <c r="F19" s="2" t="inlineStr">
-        <is>
-          <t>207 Trillion</t>
-        </is>
-      </c>
-      <c r="G19" s="3" t="inlineStr">
-        <is>
-          <t>206,708,435,907,937</t>
-        </is>
-      </c>
+      <c r="F19" s="2" t="n"/>
+      <c r="G19" s="2" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -1120,7 +989,7 @@
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>195,387,272,187,845</t>
+          <t>195,405,153,664,131</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
@@ -1133,16 +1002,8 @@
           <t xml:space="preserve">0.1954% </t>
         </is>
       </c>
-      <c r="F20" s="2" t="inlineStr">
-        <is>
-          <t>195 Trillion</t>
-        </is>
-      </c>
-      <c r="G20" s="3" t="inlineStr">
-        <is>
-          <t>195,387,272,187,845</t>
-        </is>
-      </c>
+      <c r="F20" s="2" t="n"/>
+      <c r="G20" s="2" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -1168,16 +1029,8 @@
           <t xml:space="preserve">0.1865% </t>
         </is>
       </c>
-      <c r="F21" s="2" t="inlineStr">
-        <is>
-          <t>187 Trillion</t>
-        </is>
-      </c>
-      <c r="G21" s="3" t="inlineStr">
-        <is>
-          <t>186,538,338,493,022</t>
-        </is>
-      </c>
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="2" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -1185,12 +1038,12 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>0xde58455ce16cb194a4dc90532326fbf9f3ba8513</t>
+          <t>0x497e289791fc2c2b355c259d9516f079d9b52a63</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>179,053,276,845,724</t>
+          <t>178,782,769,715,143</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
@@ -1200,19 +1053,11 @@
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1791% </t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>179 Trillion</t>
-        </is>
-      </c>
-      <c r="G22" s="3" t="inlineStr">
-        <is>
-          <t>179,053,276,845,724</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1788% </t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="2" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -1220,34 +1065,26 @@
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>0x497e289791fc2c2b355c259d9516f079d9b52a63</t>
+          <t>0x4159fcaefd2216a1b581587ca97da9f53e8ba163</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>178,782,769,715,143</t>
+          <t>170,950,814,651,786</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>179 Trillion</t>
+          <t>171 Trillion</t>
         </is>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1788% </t>
-        </is>
-      </c>
-      <c r="F23" s="2" t="inlineStr">
-        <is>
-          <t>179 Trillion</t>
-        </is>
-      </c>
-      <c r="G23" s="3" t="inlineStr">
-        <is>
-          <t>178,782,769,715,143</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1710% </t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="n"/>
+      <c r="G23" s="2" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -1255,12 +1092,12 @@
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>0x4159fcaefd2216a1b581587ca97da9f53e8ba163</t>
+          <t>0xf3f83f6a5830e55b45b3c44010be0481baa1b9be</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>170,924,102,105,501</t>
+          <t>170,558,414,075,509</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
@@ -1270,52 +1107,44 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1709% </t>
-        </is>
-      </c>
-      <c r="F24" s="2" t="inlineStr">
-        <is>
-          <t>171 Trillion</t>
-        </is>
-      </c>
-      <c r="G24" s="3" t="inlineStr">
-        <is>
-          <t>170,924,102,105,501</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1706% </t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="n"/>
+      <c r="G24" s="2" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <t>0xf3f83f6a5830e55b45b3c44010be0481baa1b9be</t>
-        </is>
-      </c>
-      <c r="C25" s="3" t="inlineStr">
-        <is>
-          <t>170,324,308,669,562</t>
-        </is>
-      </c>
-      <c r="D25" s="3" t="inlineStr">
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>0xd693658b31ef059354118ac2b8067b989ebf4b2b</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>170,382,155,915,106</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="inlineStr">
         <is>
           <t>170 Trillion</t>
         </is>
       </c>
-      <c r="E25" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1703% </t>
-        </is>
-      </c>
-      <c r="F25" s="2" t="inlineStr">
-        <is>
-          <t>170 Trillion</t>
-        </is>
-      </c>
-      <c r="G25" s="3" t="inlineStr">
-        <is>
-          <t>170,324,308,669,562</t>
+      <c r="E25" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1704% </t>
+        </is>
+      </c>
+      <c r="F25" s="4" t="inlineStr">
+        <is>
+          <t>3 Trillion More</t>
+        </is>
+      </c>
+      <c r="G25" s="5" t="inlineStr">
+        <is>
+          <t>3,046,627,653,209</t>
         </is>
       </c>
     </row>
@@ -1325,34 +1154,26 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>0xd693658b31ef059354118ac2b8067b989ebf4b2b</t>
+          <t>0xbdf119001cf9d44d902bf7d8e283e10ab66ddeea</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>167,335,528,261,897</t>
+          <t>160,512,332,157,587</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>167 Trillion</t>
+          <t>161 Trillion</t>
         </is>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1673% </t>
-        </is>
-      </c>
-      <c r="F26" s="2" t="inlineStr">
-        <is>
-          <t>167 Trillion</t>
-        </is>
-      </c>
-      <c r="G26" s="3" t="inlineStr">
-        <is>
-          <t>167,335,528,261,897</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1605% </t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="n"/>
+      <c r="G26" s="2" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -1360,34 +1181,26 @@
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>0xbdf119001cf9d44d902bf7d8e283e10ab66ddeea</t>
+          <t>0xcc6833974ce5970eac45e7751573c30c7b41a4a5</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>160,512,332,157,587</t>
+          <t>156,599,878,119,906</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t>161 Trillion</t>
+          <t>157 Trillion</t>
         </is>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1605% </t>
-        </is>
-      </c>
-      <c r="F27" s="2" t="inlineStr">
-        <is>
-          <t>161 Trillion</t>
-        </is>
-      </c>
-      <c r="G27" s="3" t="inlineStr">
-        <is>
-          <t>160,512,332,157,587</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1566% </t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="n"/>
+      <c r="G27" s="2" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -1395,34 +1208,26 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>0xcc6833974ce5970eac45e7751573c30c7b41a4a5</t>
+          <t>0x7b5b9b8d134bec76023cd6c20358d38714cc5c58</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>156,599,878,119,906</t>
+          <t>152,751,853,489,352</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>157 Trillion</t>
+          <t>153 Trillion</t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1566% </t>
-        </is>
-      </c>
-      <c r="F28" s="2" t="inlineStr">
-        <is>
-          <t>157 Trillion</t>
-        </is>
-      </c>
-      <c r="G28" s="3" t="inlineStr">
-        <is>
-          <t>156,599,878,119,906</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1528% </t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="n"/>
+      <c r="G28" s="2" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
@@ -1430,34 +1235,26 @@
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>0x7b5b9b8d134bec76023cd6c20358d38714cc5c58</t>
+          <t>0x1ae48253b364374d3db52de311302fc501b87895</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>152,751,853,489,352</t>
+          <t>152,401,926,728,651</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>153 Trillion</t>
+          <t>152 Trillion</t>
         </is>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1528% </t>
-        </is>
-      </c>
-      <c r="F29" s="2" t="inlineStr">
-        <is>
-          <t>153 Trillion</t>
-        </is>
-      </c>
-      <c r="G29" s="3" t="inlineStr">
-        <is>
-          <t>152,751,853,489,352</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1524% </t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="n"/>
+      <c r="G29" s="2" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -1465,34 +1262,26 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>0x1ae48253b364374d3db52de311302fc501b87895</t>
+          <t>0x9a7e16cc5d152e60ea52d46d8e422d724bdb4dcf</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>152,401,926,728,651</t>
+          <t>150,058,675,230,722</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>152 Trillion</t>
+          <t>150 Trillion</t>
         </is>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1524% </t>
-        </is>
-      </c>
-      <c r="F30" s="2" t="inlineStr">
-        <is>
-          <t>152 Trillion</t>
-        </is>
-      </c>
-      <c r="G30" s="3" t="inlineStr">
-        <is>
-          <t>152,401,926,728,651</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1501% </t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="2" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
@@ -1500,34 +1289,26 @@
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>0x9a7e16cc5d152e60ea52d46d8e422d724bdb4dcf</t>
+          <t>0x672c36fa22029369490bb5e33e6d16a7e1309c1e</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>150,011,755,571,316</t>
+          <t>141,084,704,642,644</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
         <is>
-          <t>150 Trillion</t>
+          <t>141 Trillion</t>
         </is>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1500% </t>
-        </is>
-      </c>
-      <c r="F31" s="2" t="inlineStr">
-        <is>
-          <t>150 Trillion</t>
-        </is>
-      </c>
-      <c r="G31" s="3" t="inlineStr">
-        <is>
-          <t>150,011,755,571,316</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1411% </t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="n"/>
+      <c r="G31" s="2" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -1535,34 +1316,26 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>0x672c36fa22029369490bb5e33e6d16a7e1309c1e</t>
+          <t>0x6111742b05e8ece0d9fedb82bcfdc597be7b43d9</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>141,084,704,642,644</t>
+          <t>137,943,162,320,277</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>141 Trillion</t>
+          <t>138 Trillion</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1411% </t>
-        </is>
-      </c>
-      <c r="F32" s="2" t="inlineStr">
-        <is>
-          <t>141 Trillion</t>
-        </is>
-      </c>
-      <c r="G32" s="3" t="inlineStr">
-        <is>
-          <t>141,084,704,642,644</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1379% </t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="n"/>
+      <c r="G32" s="2" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
@@ -1570,34 +1343,26 @@
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>0x6111742b05e8ece0d9fedb82bcfdc597be7b43d9</t>
+          <t>0x3d268cd580f89cfe6cc5dcf8764f51085f74a649</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>137,943,162,320,277</t>
+          <t>127,831,467,781,837</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>138 Trillion</t>
+          <t>128 Trillion</t>
         </is>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1379% </t>
-        </is>
-      </c>
-      <c r="F33" s="2" t="inlineStr">
-        <is>
-          <t>138 Trillion</t>
-        </is>
-      </c>
-      <c r="G33" s="3" t="inlineStr">
-        <is>
-          <t>137,943,162,320,277</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1278% </t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="n"/>
+      <c r="G33" s="2" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -1605,34 +1370,26 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>0x3d268cd580f89cfe6cc5dcf8764f51085f74a649</t>
+          <t>0x30e9bda3cefff54d93fd5954b1961b8a5fea03e2</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>127,831,467,781,837</t>
+          <t>126,954,615,749,228</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>128 Trillion</t>
+          <t>127 Trillion</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1278% </t>
-        </is>
-      </c>
-      <c r="F34" s="2" t="inlineStr">
-        <is>
-          <t>128 Trillion</t>
-        </is>
-      </c>
-      <c r="G34" s="3" t="inlineStr">
-        <is>
-          <t>127,831,467,781,837</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1270% </t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="n"/>
+      <c r="G34" s="2" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
@@ -1640,34 +1397,26 @@
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>0x30e9bda3cefff54d93fd5954b1961b8a5fea03e2</t>
+          <t>0xa9adda56845662af63a16a02afe2512e0babe4f0</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>126,654,677,093,340</t>
+          <t>125,102,299,894,734</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>127 Trillion</t>
+          <t>125 Trillion</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1267% </t>
-        </is>
-      </c>
-      <c r="F35" s="2" t="inlineStr">
-        <is>
-          <t>127 Trillion</t>
-        </is>
-      </c>
-      <c r="G35" s="3" t="inlineStr">
-        <is>
-          <t>126,654,677,093,340</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1251% </t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="n"/>
+      <c r="G35" s="2" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -1675,34 +1424,26 @@
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>0xa9adda56845662af63a16a02afe2512e0babe4f0</t>
+          <t>0xf076f6f942eac10b48cea9ed1f25be813304ae42</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>125,102,299,894,734</t>
+          <t>116,910,581,367,992</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
         <is>
-          <t>125 Trillion</t>
+          <t>117 Trillion</t>
         </is>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1251% </t>
-        </is>
-      </c>
-      <c r="F36" s="2" t="inlineStr">
-        <is>
-          <t>125 Trillion</t>
-        </is>
-      </c>
-      <c r="G36" s="3" t="inlineStr">
-        <is>
-          <t>125,102,299,894,734</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1169% </t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="n"/>
+      <c r="G36" s="2" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
@@ -1710,34 +1451,26 @@
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>0xf076f6f942eac10b48cea9ed1f25be813304ae42</t>
+          <t>0x8117f26ab0e42ccae6009bd48675e2cdc94e95b6</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>116,910,581,367,992</t>
+          <t>115,770,730,436,412</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
         <is>
-          <t>117 Trillion</t>
+          <t>116 Trillion</t>
         </is>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1169% </t>
-        </is>
-      </c>
-      <c r="F37" s="2" t="inlineStr">
-        <is>
-          <t>117 Trillion</t>
-        </is>
-      </c>
-      <c r="G37" s="3" t="inlineStr">
-        <is>
-          <t>116,910,581,367,992</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1158% </t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="n"/>
+      <c r="G37" s="2" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
@@ -1745,12 +1478,12 @@
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>0x8117f26ab0e42ccae6009bd48675e2cdc94e95b6</t>
+          <t>0x74beaeb59500b4486ec3c83b81552279b79c6728</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>115,397,010,893,158</t>
+          <t>115,059,068,116,820</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
@@ -1760,19 +1493,11 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1154% </t>
-        </is>
-      </c>
-      <c r="F38" s="2" t="inlineStr">
-        <is>
-          <t>115 Trillion</t>
-        </is>
-      </c>
-      <c r="G38" s="3" t="inlineStr">
-        <is>
-          <t>115,397,010,893,158</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1151% </t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="n"/>
+      <c r="G38" s="2" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
@@ -1780,34 +1505,26 @@
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>0x74beaeb59500b4486ec3c83b81552279b79c6728</t>
+          <t>0x493d3d63b6e92869098d3ce8d733ce220633b829</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>115,053,018,428,491</t>
+          <t>110,825,174,828,856</t>
         </is>
       </c>
       <c r="D39" s="3" t="inlineStr">
         <is>
-          <t>115 Trillion</t>
+          <t>111 Trillion</t>
         </is>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1151% </t>
-        </is>
-      </c>
-      <c r="F39" s="2" t="inlineStr">
-        <is>
-          <t>115 Trillion</t>
-        </is>
-      </c>
-      <c r="G39" s="3" t="inlineStr">
-        <is>
-          <t>115,053,018,428,491</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1108% </t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="n"/>
+      <c r="G39" s="2" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -1815,34 +1532,26 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>0x493d3d63b6e92869098d3ce8d733ce220633b829</t>
+          <t>0x3efbd5727056766f2023a132d3de638b8e9bcf00</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>110,722,477,971,006</t>
+          <t>109,231,111,388,513</t>
         </is>
       </c>
       <c r="D40" s="3" t="inlineStr">
         <is>
-          <t>111 Trillion</t>
+          <t>109 Trillion</t>
         </is>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1107% </t>
-        </is>
-      </c>
-      <c r="F40" s="2" t="inlineStr">
-        <is>
-          <t>111 Trillion</t>
-        </is>
-      </c>
-      <c r="G40" s="3" t="inlineStr">
-        <is>
-          <t>110,722,477,971,006</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1092% </t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="n"/>
+      <c r="G40" s="2" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
@@ -1850,34 +1559,26 @@
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>0x3efbd5727056766f2023a132d3de638b8e9bcf00</t>
+          <t>0xb2c5ae080a236fe89a87fdbd1f9d58ad4b57c6b2</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>109,164,258,864,218</t>
+          <t>107,359,482,135,805</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
         <is>
-          <t>109 Trillion</t>
+          <t>107 Trillion</t>
         </is>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1092% </t>
-        </is>
-      </c>
-      <c r="F41" s="2" t="inlineStr">
-        <is>
-          <t>109 Trillion</t>
-        </is>
-      </c>
-      <c r="G41" s="3" t="inlineStr">
-        <is>
-          <t>109,164,258,864,218</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1074% </t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="n"/>
+      <c r="G41" s="2" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -1885,34 +1586,26 @@
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>0xb2c5ae080a236fe89a87fdbd1f9d58ad4b57c6b2</t>
+          <t>0x68bae0996364afaa2240f17c2055da0e12193337</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
         <is>
-          <t>107,231,043,642,629</t>
+          <t>105,551,878,645,914</t>
         </is>
       </c>
       <c r="D42" s="3" t="inlineStr">
         <is>
-          <t>107 Trillion</t>
+          <t>106 Trillion</t>
         </is>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1072% </t>
-        </is>
-      </c>
-      <c r="F42" s="2" t="inlineStr">
-        <is>
-          <t>107 Trillion</t>
-        </is>
-      </c>
-      <c r="G42" s="3" t="inlineStr">
-        <is>
-          <t>107,231,043,642,629</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1056% </t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="n"/>
+      <c r="G42" s="2" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -1920,67 +1613,59 @@
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>0x68bae0996364afaa2240f17c2055da0e12193337</t>
+          <t>0xa4fd3063a3d831801c7791b5de3fb9e7a5dcbe23</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>105,528,268,631,327</t>
+          <t>102,426,922,337,291</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>106 Trillion</t>
+          <t>102 Trillion</t>
         </is>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1055% </t>
-        </is>
-      </c>
-      <c r="F43" s="2" t="inlineStr">
-        <is>
-          <t>106 Trillion</t>
-        </is>
-      </c>
-      <c r="G43" s="3" t="inlineStr">
-        <is>
-          <t>105,528,268,631,327</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1024% </t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="n"/>
+      <c r="G43" s="2" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="n">
+      <c r="A44" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="inlineStr">
-        <is>
-          <t>0xa4fd3063a3d831801c7791b5de3fb9e7a5dcbe23</t>
-        </is>
-      </c>
-      <c r="C44" s="3" t="inlineStr">
-        <is>
-          <t>102,364,311,646,270</t>
-        </is>
-      </c>
-      <c r="D44" s="3" t="inlineStr">
+      <c r="B44" s="4" t="inlineStr">
+        <is>
+          <t>0xde58455ce16cb194a4dc90532326fbf9f3ba8513</t>
+        </is>
+      </c>
+      <c r="C44" s="5" t="inlineStr">
+        <is>
+          <t>102,064,655,233,239</t>
+        </is>
+      </c>
+      <c r="D44" s="5" t="inlineStr">
         <is>
           <t>102 Trillion</t>
         </is>
       </c>
-      <c r="E44" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1024% </t>
-        </is>
-      </c>
-      <c r="F44" s="2" t="inlineStr">
-        <is>
-          <t>102 Trillion</t>
-        </is>
-      </c>
-      <c r="G44" s="3" t="inlineStr">
-        <is>
-          <t>102,364,311,646,270</t>
+      <c r="E44" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1021% </t>
+        </is>
+      </c>
+      <c r="F44" s="6" t="inlineStr">
+        <is>
+          <t>77 Trillion Less</t>
+        </is>
+      </c>
+      <c r="G44" s="7" t="inlineStr">
+        <is>
+          <t>76,988,621,612,485</t>
         </is>
       </c>
     </row>
@@ -1995,7 +1680,7 @@
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>101,585,280,597,533</t>
+          <t>101,678,788,166,514</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
@@ -2005,19 +1690,11 @@
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1016% </t>
-        </is>
-      </c>
-      <c r="F45" s="2" t="inlineStr">
-        <is>
-          <t>102 Trillion</t>
-        </is>
-      </c>
-      <c r="G45" s="3" t="inlineStr">
-        <is>
-          <t>101,585,280,597,533</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1017% </t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="n"/>
+      <c r="G45" s="2" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
@@ -2030,7 +1707,7 @@
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>101,057,776,636,998</t>
+          <t>101,119,599,269,434</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
@@ -2043,16 +1720,8 @@
           <t xml:space="preserve">0.1011% </t>
         </is>
       </c>
-      <c r="F46" s="2" t="inlineStr">
-        <is>
-          <t>101 Trillion</t>
-        </is>
-      </c>
-      <c r="G46" s="3" t="inlineStr">
-        <is>
-          <t>101,057,776,636,998</t>
-        </is>
-      </c>
+      <c r="F46" s="2" t="n"/>
+      <c r="G46" s="2" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
@@ -2065,7 +1734,7 @@
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>100,948,140,780,737</t>
+          <t>100,961,617,021,611</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
@@ -2075,19 +1744,11 @@
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1009% </t>
-        </is>
-      </c>
-      <c r="F47" s="2" t="inlineStr">
-        <is>
-          <t>101 Trillion</t>
-        </is>
-      </c>
-      <c r="G47" s="3" t="inlineStr">
-        <is>
-          <t>100,948,140,780,737</t>
-        </is>
-      </c>
+          <t xml:space="preserve">0.1010% </t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="n"/>
+      <c r="G47" s="2" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -2100,7 +1761,7 @@
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>100,369,561,229,078</t>
+          <t>100,372,973,911,978</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
@@ -2113,16 +1774,8 @@
           <t xml:space="preserve">0.1004% </t>
         </is>
       </c>
-      <c r="F48" s="2" t="inlineStr">
-        <is>
-          <t>100 Trillion</t>
-        </is>
-      </c>
-      <c r="G48" s="3" t="inlineStr">
-        <is>
-          <t>100,369,561,229,078</t>
-        </is>
-      </c>
+      <c r="F48" s="2" t="n"/>
+      <c r="G48" s="2" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
@@ -2130,54 +1783,56 @@
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>0x505dd22c1bacced7531f319f5008318a440490bc</t>
+          <t>0x302c44b648f5a84191f08551be26a2d2456a1fa1</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>95,004,246,973,923</t>
+          <t>92,530,224,244,054</t>
         </is>
       </c>
       <c r="D49" s="3" t="inlineStr">
         <is>
-          <t>95 Trillion</t>
+          <t>93 Trillion</t>
         </is>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0950% </t>
-        </is>
-      </c>
-      <c r="F49" s="2" t="inlineStr">
-        <is>
-          <t>95 Trillion</t>
-        </is>
-      </c>
-      <c r="G49" s="3" t="inlineStr">
-        <is>
-          <t>95,004,246,973,923</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" s="4" t="inlineStr">
+          <t xml:space="preserve">0.0925% </t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="n"/>
+      <c r="G49" s="2" t="n"/>
+    </row>
+    <row r="53">
+      <c r="B53" s="3" t="inlineStr">
         <is>
           <t>Total's</t>
         </is>
       </c>
-      <c r="C51" s="4" t="inlineStr">
-        <is>
-          <t>12,156,605,285,967,305</t>
-        </is>
-      </c>
-      <c r="D51" s="4" t="inlineStr">
-        <is>
-          <t>12157 Trillion</t>
-        </is>
-      </c>
-      <c r="E51" s="4" t="inlineStr">
-        <is>
-          <t>12.16%</t>
+      <c r="C53" s="3" t="inlineStr">
+        <is>
+          <t>12,082,313,291,653,367</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
+          <t>12082 Trillion</t>
+        </is>
+      </c>
+      <c r="E53" s="3" t="inlineStr">
+        <is>
+          <t>12.08%</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>-74 Trillion</t>
+        </is>
+      </c>
+      <c r="G53" s="2" t="inlineStr">
+        <is>
+          <t>-73,941,993,959,276</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix old holder file
</commit_message>
<xml_diff>
--- a/WhaleWatching/holders.xlsx
+++ b/WhaleWatching/holders.xlsx
@@ -795,22 +795,22 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>0x69fe97ce030074b37cbaf3ee46e9f68ca8712099</t>
+          <t>0x7167d70b2e6b167633356254bf22f5d32aedcd5b</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>406,746,124,267,053</t>
+          <t>405,964,100,208,639</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>407 Trillion</t>
+          <t>406 Trillion</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4067% </t>
+          <t xml:space="preserve">0.4060% </t>
         </is>
       </c>
       <c r="F13" s="2" t="n"/>
@@ -822,53 +822,61 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>0x7167d70b2e6b167633356254bf22f5d32aedcd5b</t>
+          <t>0x7395cb62e4405b6c1174c2329f444af6ee7bdfd9</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>405,964,100,208,639</t>
+          <t>362,521,477,411,729</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>406 Trillion</t>
+          <t>363 Trillion</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4060% </t>
+          <t xml:space="preserve">0.3625% </t>
         </is>
       </c>
       <c r="F14" s="2" t="n"/>
       <c r="G14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>0x7395cb62e4405b6c1174c2329f444af6ee7bdfd9</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>362,521,477,411,729</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>363 Trillion</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.3625% </t>
-        </is>
-      </c>
-      <c r="F15" s="2" t="n"/>
-      <c r="G15" s="2" t="n"/>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>0x69fe97ce030074b37cbaf3ee46e9f68ca8712099</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>360,003,463,717,642</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="inlineStr">
+        <is>
+          <t>360 Trillion</t>
+        </is>
+      </c>
+      <c r="E15" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.3600% </t>
+        </is>
+      </c>
+      <c r="F15" s="6" t="inlineStr">
+        <is>
+          <t>47 Trillion Less</t>
+        </is>
+      </c>
+      <c r="G15" s="7" t="inlineStr">
+        <is>
+          <t>46,742,660,549,411</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -1097,7 +1105,7 @@
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>170,558,414,075,509</t>
+          <t>170,559,005,253,847</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
@@ -1114,39 +1122,31 @@
       <c r="G24" s="2" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n">
+      <c r="A25" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>0xd693658b31ef059354118ac2b8067b989ebf4b2b</t>
         </is>
       </c>
-      <c r="C25" s="5" t="inlineStr">
+      <c r="C25" s="3" t="inlineStr">
         <is>
           <t>170,382,155,915,106</t>
         </is>
       </c>
-      <c r="D25" s="5" t="inlineStr">
+      <c r="D25" s="3" t="inlineStr">
         <is>
           <t>170 Trillion</t>
         </is>
       </c>
-      <c r="E25" s="5" t="inlineStr">
+      <c r="E25" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">0.1704% </t>
         </is>
       </c>
-      <c r="F25" s="4" t="inlineStr">
-        <is>
-          <t>3 Trillion More</t>
-        </is>
-      </c>
-      <c r="G25" s="5" t="inlineStr">
-        <is>
-          <t>3,046,627,653,209</t>
-        </is>
-      </c>
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="2" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -1635,39 +1635,31 @@
       <c r="G43" s="2" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="n">
+      <c r="A44" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="4" t="inlineStr">
+      <c r="B44" s="2" t="inlineStr">
         <is>
           <t>0xde58455ce16cb194a4dc90532326fbf9f3ba8513</t>
         </is>
       </c>
-      <c r="C44" s="5" t="inlineStr">
+      <c r="C44" s="3" t="inlineStr">
         <is>
           <t>102,064,655,233,239</t>
         </is>
       </c>
-      <c r="D44" s="5" t="inlineStr">
+      <c r="D44" s="3" t="inlineStr">
         <is>
           <t>102 Trillion</t>
         </is>
       </c>
-      <c r="E44" s="5" t="inlineStr">
+      <c r="E44" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">0.1021% </t>
         </is>
       </c>
-      <c r="F44" s="6" t="inlineStr">
-        <is>
-          <t>77 Trillion Less</t>
-        </is>
-      </c>
-      <c r="G44" s="7" t="inlineStr">
-        <is>
-          <t>76,988,621,612,485</t>
-        </is>
-      </c>
+      <c r="F44" s="2" t="n"/>
+      <c r="G44" s="2" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -1812,27 +1804,27 @@
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>12,082,313,291,653,367</t>
+          <t>12,035,571,222,282,294</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
         <is>
-          <t>12082 Trillion</t>
+          <t>12036 Trillion</t>
         </is>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>12.08%</t>
+          <t>12.04%</t>
         </is>
       </c>
       <c r="F53" s="2" t="inlineStr">
         <is>
-          <t>-74 Trillion</t>
+          <t>-47 Trillion</t>
         </is>
       </c>
       <c r="G53" s="2" t="inlineStr">
         <is>
-          <t>-73,941,993,959,276</t>
+          <t>-46,742,660,549,411</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add old whale balance finder
</commit_message>
<xml_diff>
--- a/WhaleWatching/holders.xlsx
+++ b/WhaleWatching/holders.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>760,733,598,377,011</t>
+          <t>761,082,598,387,042</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.7607% </t>
+          <t xml:space="preserve">0.7611% </t>
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
@@ -530,7 +530,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>755,805,960,029,718</t>
+          <t>756,107,607,679,423</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.7558% </t>
+          <t xml:space="preserve">0.7561% </t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -557,7 +557,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>603,712,409,699,892</t>
+          <t>603,980,172,214,805</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.6037% </t>
+          <t xml:space="preserve">0.6040% </t>
         </is>
       </c>
       <c r="F4" s="2" t="n"/>
@@ -584,7 +584,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>602,530,791,527,282</t>
+          <t>602,821,058,845,833</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -594,38 +594,46 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.6025% </t>
+          <t xml:space="preserve">0.6028% </t>
         </is>
       </c>
       <c r="F5" s="2" t="n"/>
       <c r="G5" s="2" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>0x2bd6997bf6fcfde139eb1b9346fbf79defd4e8cc</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>549,698,341,865,050</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>550 Trillion</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.5497% </t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="n"/>
-      <c r="G6" s="2" t="n"/>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>0xcdc162e71e7517e94c0c72de16ca6315349d47fc</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>529,250,426,560,027</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>529 Trillion</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.5293% </t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>29 Trillion More</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>28,955,311,081,981</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -638,7 +646,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>524,146,288,497,680</t>
+          <t>524,355,454,029,402</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
@@ -648,7 +656,7 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.5241% </t>
+          <t xml:space="preserve">0.5244% </t>
         </is>
       </c>
       <c r="F7" s="2" t="n"/>
@@ -660,22 +668,22 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>0xcdc162e71e7517e94c0c72de16ca6315349d47fc</t>
+          <t>0x7fcc2410d49222563a5cd46c0ceaffb72cf195d4</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>500,342,304,983,551</t>
+          <t>432,594,179,759,658</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>500 Trillion</t>
+          <t>433 Trillion</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.5003% </t>
+          <t xml:space="preserve">0.4326% </t>
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
@@ -687,22 +695,22 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>0x7fcc2410d49222563a5cd46c0ceaffb72cf195d4</t>
+          <t>0xac3e1d277c3442ac1c695a369d87004aed308a7d</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>432,439,854,928,747</t>
+          <t>419,994,932,243,674</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>432 Trillion</t>
+          <t>420 Trillion</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4324% </t>
+          <t xml:space="preserve">0.4200% </t>
         </is>
       </c>
       <c r="F9" s="2" t="n"/>
@@ -714,22 +722,22 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>0xac3e1d277c3442ac1c695a369d87004aed308a7d</t>
+          <t>0xbd09e0594fbdbc5f73fe5db01bdc3bc2a19ec2d7</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>419,994,932,243,674</t>
+          <t>419,360,533,364,969</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>420 Trillion</t>
+          <t>419 Trillion</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4200% </t>
+          <t xml:space="preserve">0.4194% </t>
         </is>
       </c>
       <c r="F10" s="2" t="n"/>
@@ -741,22 +749,22 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>0xbd09e0594fbdbc5f73fe5db01bdc3bc2a19ec2d7</t>
+          <t>0x0932767b51f1faedc5a86fb935eec8032f62eea8</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>419,360,533,364,969</t>
+          <t>415,228,348,905,327</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>419 Trillion</t>
+          <t>415 Trillion</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4194% </t>
+          <t xml:space="preserve">0.4152% </t>
         </is>
       </c>
       <c r="F11" s="2" t="n"/>
@@ -768,22 +776,22 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>0x0932767b51f1faedc5a86fb935eec8032f62eea8</t>
+          <t>0x7167d70b2e6b167633356254bf22f5d32aedcd5b</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>415,228,348,905,327</t>
+          <t>405,513,667,501,757</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>415 Trillion</t>
+          <t>406 Trillion</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4152% </t>
+          <t xml:space="preserve">0.4055% </t>
         </is>
       </c>
       <c r="F12" s="2" t="n"/>
@@ -795,22 +803,22 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>0x7167d70b2e6b167633356254bf22f5d32aedcd5b</t>
+          <t>0x7395cb62e4405b6c1174c2329f444af6ee7bdfd9</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>405,964,100,208,639</t>
+          <t>362,521,477,411,729</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>406 Trillion</t>
+          <t>363 Trillion</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4060% </t>
+          <t xml:space="preserve">0.3625% </t>
         </is>
       </c>
       <c r="F13" s="2" t="n"/>
@@ -822,22 +830,22 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>0x7395cb62e4405b6c1174c2329f444af6ee7bdfd9</t>
+          <t>0xf7625178ef07107edc2005a0e5d2fc411573f381</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>362,521,477,411,729</t>
+          <t>357,037,237,086,702</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>363 Trillion</t>
+          <t>357 Trillion</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.3625% </t>
+          <t xml:space="preserve">0.3570% </t>
         </is>
       </c>
       <c r="F14" s="2" t="n"/>
@@ -854,27 +862,27 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>360,003,463,717,642</t>
+          <t>324,017,179,896,078</t>
         </is>
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>360 Trillion</t>
+          <t>324 Trillion</t>
         </is>
       </c>
       <c r="E15" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.3600% </t>
+          <t xml:space="preserve">0.3240% </t>
         </is>
       </c>
       <c r="F15" s="6" t="inlineStr">
         <is>
-          <t>47 Trillion Less</t>
+          <t>83 Trillion Less</t>
         </is>
       </c>
       <c r="G15" s="7" t="inlineStr">
         <is>
-          <t>46,742,660,549,411</t>
+          <t>82,728,944,370,975</t>
         </is>
       </c>
     </row>
@@ -916,7 +924,7 @@
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>250,044,900,251,963</t>
+          <t>250,088,171,286,383</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
@@ -926,38 +934,46 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.2500% </t>
+          <t xml:space="preserve">0.2501% </t>
         </is>
       </c>
       <c r="F17" s="2" t="n"/>
       <c r="G17" s="2" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>0x14dd63527333ff7269a59985658224f96faab068</t>
-        </is>
-      </c>
-      <c r="C18" s="3" t="inlineStr">
-        <is>
-          <t>217,372,420,035,141</t>
-        </is>
-      </c>
-      <c r="D18" s="3" t="inlineStr">
-        <is>
-          <t>217 Trillion</t>
-        </is>
-      </c>
-      <c r="E18" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.2174% </t>
-        </is>
-      </c>
-      <c r="F18" s="2" t="n"/>
-      <c r="G18" s="2" t="n"/>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>0x6111742b05e8ece0d9fedb82bcfdc597be7b43d9</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>232,191,361,549,013</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>232 Trillion</t>
+        </is>
+      </c>
+      <c r="E18" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.2322% </t>
+        </is>
+      </c>
+      <c r="F18" s="4" t="inlineStr">
+        <is>
+          <t>94 Trillion More</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>94,248,199,228,736</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -965,22 +981,22 @@
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>0xfdd50de023c9a705d9086bf821d15c7450ee93bf</t>
+          <t>0x14dd63527333ff7269a59985658224f96faab068</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>206,708,435,907,937</t>
+          <t>217,372,420,035,141</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>207 Trillion</t>
+          <t>217 Trillion</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.2067% </t>
+          <t xml:space="preserve">0.2174% </t>
         </is>
       </c>
       <c r="F19" s="2" t="n"/>
@@ -992,22 +1008,22 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>0x7146f34d166379b4ab5220f5eefd7c79835a3c04</t>
+          <t>0xfdd50de023c9a705d9086bf821d15c7450ee93bf</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>195,405,153,664,131</t>
+          <t>206,708,435,907,937</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>195 Trillion</t>
+          <t>207 Trillion</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1954% </t>
+          <t xml:space="preserve">0.2067% </t>
         </is>
       </c>
       <c r="F20" s="2" t="n"/>
@@ -1019,22 +1035,22 @@
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>0x73149b3cd5e1b8536747048259419147e81a71a9</t>
+          <t>0x7146f34d166379b4ab5220f5eefd7c79835a3c04</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>186,538,338,493,022</t>
+          <t>195,405,153,664,131</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>187 Trillion</t>
+          <t>195 Trillion</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1865% </t>
+          <t xml:space="preserve">0.1954% </t>
         </is>
       </c>
       <c r="F21" s="2" t="n"/>
@@ -1046,22 +1062,22 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>0x497e289791fc2c2b355c259d9516f079d9b52a63</t>
+          <t>0x7b11f31fc0d0a79717ec025d411ac5e899ac7116</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>178,782,769,715,143</t>
+          <t>192,956,295,255,817</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>179 Trillion</t>
+          <t>193 Trillion</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1788% </t>
+          <t xml:space="preserve">0.1930% </t>
         </is>
       </c>
       <c r="F22" s="2" t="n"/>
@@ -1073,53 +1089,61 @@
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>0x4159fcaefd2216a1b581587ca97da9f53e8ba163</t>
+          <t>0x73149b3cd5e1b8536747048259419147e81a71a9</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>170,950,814,651,786</t>
+          <t>186,576,038,288,042</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>171 Trillion</t>
+          <t>187 Trillion</t>
         </is>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1710% </t>
+          <t xml:space="preserve">0.1866% </t>
         </is>
       </c>
       <c r="F23" s="2" t="n"/>
       <c r="G23" s="2" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="inlineStr">
-        <is>
-          <t>0xf3f83f6a5830e55b45b3c44010be0481baa1b9be</t>
-        </is>
-      </c>
-      <c r="C24" s="3" t="inlineStr">
-        <is>
-          <t>170,559,005,253,847</t>
-        </is>
-      </c>
-      <c r="D24" s="3" t="inlineStr">
-        <is>
-          <t>171 Trillion</t>
-        </is>
-      </c>
-      <c r="E24" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1706% </t>
-        </is>
-      </c>
-      <c r="F24" s="2" t="n"/>
-      <c r="G24" s="2" t="n"/>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t>0x672c36fa22029369490bb5e33e6d16a7e1309c1e</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>181,413,020,794,868</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="inlineStr">
+        <is>
+          <t>181 Trillion</t>
+        </is>
+      </c>
+      <c r="E24" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1814% </t>
+        </is>
+      </c>
+      <c r="F24" s="4" t="inlineStr">
+        <is>
+          <t>40 Trillion More</t>
+        </is>
+      </c>
+      <c r="G24" s="5" t="inlineStr">
+        <is>
+          <t>40,328,316,152,224</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -1127,53 +1151,61 @@
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>0xd693658b31ef059354118ac2b8067b989ebf4b2b</t>
+          <t>0x497e289791fc2c2b355c259d9516f079d9b52a63</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>170,382,155,915,106</t>
+          <t>178,884,424,353,453</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
         <is>
-          <t>170 Trillion</t>
+          <t>179 Trillion</t>
         </is>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1704% </t>
+          <t xml:space="preserve">0.1789% </t>
         </is>
       </c>
       <c r="F25" s="2" t="n"/>
       <c r="G25" s="2" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="inlineStr">
-        <is>
-          <t>0xbdf119001cf9d44d902bf7d8e283e10ab66ddeea</t>
-        </is>
-      </c>
-      <c r="C26" s="3" t="inlineStr">
-        <is>
-          <t>160,512,332,157,587</t>
-        </is>
-      </c>
-      <c r="D26" s="3" t="inlineStr">
-        <is>
-          <t>161 Trillion</t>
-        </is>
-      </c>
-      <c r="E26" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1605% </t>
-        </is>
-      </c>
-      <c r="F26" s="2" t="n"/>
-      <c r="G26" s="2" t="n"/>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>0xd693658b31ef059354118ac2b8067b989ebf4b2b</t>
+        </is>
+      </c>
+      <c r="C26" s="5" t="inlineStr">
+        <is>
+          <t>172,179,198,856,685</t>
+        </is>
+      </c>
+      <c r="D26" s="5" t="inlineStr">
+        <is>
+          <t>172 Trillion</t>
+        </is>
+      </c>
+      <c r="E26" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1722% </t>
+        </is>
+      </c>
+      <c r="F26" s="4" t="inlineStr">
+        <is>
+          <t>5 Trillion More</t>
+        </is>
+      </c>
+      <c r="G26" s="5" t="inlineStr">
+        <is>
+          <t>4,843,670,594,788</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -1181,22 +1213,22 @@
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>0xcc6833974ce5970eac45e7751573c30c7b41a4a5</t>
+          <t>0xf3f83f6a5830e55b45b3c44010be0481baa1b9be</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>156,599,878,119,906</t>
+          <t>170,559,005,253,847</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t>157 Trillion</t>
+          <t>171 Trillion</t>
         </is>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1566% </t>
+          <t xml:space="preserve">0.1706% </t>
         </is>
       </c>
       <c r="F27" s="2" t="n"/>
@@ -1208,22 +1240,22 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>0x7b5b9b8d134bec76023cd6c20358d38714cc5c58</t>
+          <t>0x4159fcaefd2216a1b581587ca97da9f53e8ba163</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>152,751,853,489,352</t>
+          <t>170,029,080,849,270</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>153 Trillion</t>
+          <t>170 Trillion</t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1528% </t>
+          <t xml:space="preserve">0.1700% </t>
         </is>
       </c>
       <c r="F28" s="2" t="n"/>
@@ -1235,22 +1267,22 @@
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>0x1ae48253b364374d3db52de311302fc501b87895</t>
+          <t>0xbdf119001cf9d44d902bf7d8e283e10ab66ddeea</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>152,401,926,728,651</t>
+          <t>160,512,332,157,587</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>152 Trillion</t>
+          <t>161 Trillion</t>
         </is>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1524% </t>
+          <t xml:space="preserve">0.1605% </t>
         </is>
       </c>
       <c r="F29" s="2" t="n"/>
@@ -1262,22 +1294,22 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>0x9a7e16cc5d152e60ea52d46d8e422d724bdb4dcf</t>
+          <t>0xcc6833974ce5970eac45e7751573c30c7b41a4a5</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>150,058,675,230,722</t>
+          <t>156,638,608,730,399</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>150 Trillion</t>
+          <t>157 Trillion</t>
         </is>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1501% </t>
+          <t xml:space="preserve">0.1566% </t>
         </is>
       </c>
       <c r="F30" s="2" t="n"/>
@@ -1289,22 +1321,22 @@
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>0x672c36fa22029369490bb5e33e6d16a7e1309c1e</t>
+          <t>0x7b5b9b8d134bec76023cd6c20358d38714cc5c58</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>141,084,704,642,644</t>
+          <t>152,751,853,489,352</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
         <is>
-          <t>141 Trillion</t>
+          <t>153 Trillion</t>
         </is>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1411% </t>
+          <t xml:space="preserve">0.1528% </t>
         </is>
       </c>
       <c r="F31" s="2" t="n"/>
@@ -1316,22 +1348,22 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>0x6111742b05e8ece0d9fedb82bcfdc597be7b43d9</t>
+          <t>0x1ae48253b364374d3db52de311302fc501b87895</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>137,943,162,320,277</t>
+          <t>152,401,926,728,651</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>138 Trillion</t>
+          <t>152 Trillion</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1379% </t>
+          <t xml:space="preserve">0.1524% </t>
         </is>
       </c>
       <c r="F32" s="2" t="n"/>
@@ -1343,22 +1375,22 @@
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>0x3d268cd580f89cfe6cc5dcf8764f51085f74a649</t>
+          <t>0x9a7e16cc5d152e60ea52d46d8e422d724bdb4dcf</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>127,831,467,781,837</t>
+          <t>150,058,675,230,722</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>128 Trillion</t>
+          <t>150 Trillion</t>
         </is>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1278% </t>
+          <t xml:space="preserve">0.1501% </t>
         </is>
       </c>
       <c r="F33" s="2" t="n"/>
@@ -1635,31 +1667,39 @@
       <c r="G43" s="2" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="n">
+      <c r="A44" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="inlineStr">
+      <c r="B44" s="4" t="inlineStr">
         <is>
           <t>0xde58455ce16cb194a4dc90532326fbf9f3ba8513</t>
         </is>
       </c>
-      <c r="C44" s="3" t="inlineStr">
+      <c r="C44" s="5" t="inlineStr">
         <is>
           <t>102,064,655,233,239</t>
         </is>
       </c>
-      <c r="D44" s="3" t="inlineStr">
+      <c r="D44" s="5" t="inlineStr">
         <is>
           <t>102 Trillion</t>
         </is>
       </c>
-      <c r="E44" s="3" t="inlineStr">
+      <c r="E44" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">0.1021% </t>
         </is>
       </c>
-      <c r="F44" s="2" t="n"/>
-      <c r="G44" s="2" t="n"/>
+      <c r="F44" s="6" t="inlineStr">
+        <is>
+          <t>77 Trillion Less</t>
+        </is>
+      </c>
+      <c r="G44" s="7" t="inlineStr">
+        <is>
+          <t>76,988,621,612,485</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -1775,22 +1815,22 @@
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>0x302c44b648f5a84191f08551be26a2d2456a1fa1</t>
+          <t>0x86437c0875fa78dc98c57bc010ef4ad07bc01715</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>92,530,224,244,054</t>
+          <t>100,127,887,461,980</t>
         </is>
       </c>
       <c r="D49" s="3" t="inlineStr">
         <is>
-          <t>93 Trillion</t>
+          <t>100 Trillion</t>
         </is>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0925% </t>
+          <t xml:space="preserve">0.1001% </t>
         </is>
       </c>
       <c r="F49" s="2" t="n"/>
@@ -1804,27 +1844,27 @@
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>12,035,571,222,282,294</t>
+          <t>12,045,349,361,697,981</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
         <is>
-          <t>12036 Trillion</t>
+          <t>12045 Trillion</t>
         </is>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>12.04%</t>
+          <t>12.05%</t>
         </is>
       </c>
       <c r="F53" s="2" t="inlineStr">
         <is>
-          <t>-47 Trillion</t>
+          <t>9 Trillion</t>
         </is>
       </c>
       <c r="G53" s="2" t="inlineStr">
         <is>
-          <t>-46,742,660,549,411</t>
+          <t>8,657,931,074,269</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add old whale tracking
</commit_message>
<xml_diff>
--- a/WhaleWatching/holders.xlsx
+++ b/WhaleWatching/holders.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -39,6 +39,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00D8D8D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ABABAB"/>
       </patternFill>
     </fill>
   </fills>
@@ -60,7 +65,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -76,6 +81,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,7 +503,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
@@ -503,7 +512,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>761,082,598,387,042</t>
+          <t>761,124,453,308,702</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -521,7 +530,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
@@ -530,7 +539,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>756,107,607,679,423</t>
+          <t>756,193,608,270,292</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -540,7 +549,7 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.7561% </t>
+          <t xml:space="preserve">0.7562% </t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -548,7 +557,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
@@ -557,7 +566,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>603,980,172,214,805</t>
+          <t>604,006,555,483,506</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -575,7 +584,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
@@ -584,7 +593,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>602,821,058,845,833</t>
+          <t>602,861,767,776,486</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -594,7 +603,7 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.6028% </t>
+          <t xml:space="preserve">0.6029% </t>
         </is>
       </c>
       <c r="F5" s="2" t="n"/>
@@ -602,7 +611,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
@@ -611,7 +620,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>529,250,426,560,027</t>
+          <t>529,273,233,399,985</t>
         </is>
       </c>
       <c r="D6" s="5" t="inlineStr">
@@ -631,13 +640,13 @@
       </c>
       <c r="G6" s="5" t="inlineStr">
         <is>
-          <t>28,955,311,081,981</t>
+          <t>28,978,117,921,939</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
@@ -664,7 +673,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
@@ -691,7 +700,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
@@ -700,7 +709,7 @@
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>419,994,932,243,674</t>
+          <t>420,029,625,185,313</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
@@ -718,7 +727,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
@@ -745,7 +754,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
@@ -772,7 +781,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
@@ -781,7 +790,7 @@
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>405,513,667,501,757</t>
+          <t>405,519,308,866,693</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
@@ -799,7 +808,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
@@ -826,7 +835,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
@@ -835,7 +844,7 @@
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>357,037,237,086,702</t>
+          <t>357,042,139,209,204</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
@@ -853,7 +862,7 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
@@ -862,7 +871,7 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>324,017,179,896,078</t>
+          <t>324,124,491,526,496</t>
         </is>
       </c>
       <c r="D15" s="5" t="inlineStr">
@@ -872,7 +881,7 @@
       </c>
       <c r="E15" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.3240% </t>
+          <t xml:space="preserve">0.3241% </t>
         </is>
       </c>
       <c r="F15" s="6" t="inlineStr">
@@ -882,13 +891,13 @@
       </c>
       <c r="G15" s="7" t="inlineStr">
         <is>
-          <t>82,728,944,370,975</t>
+          <t>82,621,632,740,557</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
@@ -915,7 +924,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
@@ -942,7 +951,7 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
@@ -951,33 +960,33 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>232,191,361,549,013</t>
+          <t>226,872,477,762,525</t>
         </is>
       </c>
       <c r="D18" s="5" t="inlineStr">
         <is>
-          <t>232 Trillion</t>
+          <t>227 Trillion</t>
         </is>
       </c>
       <c r="E18" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.2322% </t>
+          <t xml:space="preserve">0.2269% </t>
         </is>
       </c>
       <c r="F18" s="4" t="inlineStr">
         <is>
-          <t>94 Trillion More</t>
+          <t>89 Trillion More</t>
         </is>
       </c>
       <c r="G18" s="5" t="inlineStr">
         <is>
-          <t>94,248,199,228,736</t>
+          <t>88,929,315,442,248</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
@@ -1004,7 +1013,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
@@ -1013,7 +1022,7 @@
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>206,708,435,907,937</t>
+          <t>206,835,549,683,992</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
@@ -1023,7 +1032,7 @@
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.2067% </t>
+          <t xml:space="preserve">0.2068% </t>
         </is>
       </c>
       <c r="F20" s="2" t="n"/>
@@ -1031,7 +1040,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
@@ -1058,7 +1067,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
@@ -1067,7 +1076,7 @@
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>192,956,295,255,817</t>
+          <t>193,018,756,847,832</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
@@ -1085,7 +1094,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
@@ -1112,7 +1121,7 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
@@ -1147,7 +1156,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
@@ -1173,62 +1182,54 @@
       <c r="G25" s="2" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4" t="inlineStr">
-        <is>
-          <t>0xd693658b31ef059354118ac2b8067b989ebf4b2b</t>
-        </is>
-      </c>
-      <c r="C26" s="5" t="inlineStr">
-        <is>
-          <t>172,179,198,856,685</t>
-        </is>
-      </c>
-      <c r="D26" s="5" t="inlineStr">
-        <is>
-          <t>172 Trillion</t>
-        </is>
-      </c>
-      <c r="E26" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1722% </t>
-        </is>
-      </c>
-      <c r="F26" s="4" t="inlineStr">
-        <is>
-          <t>5 Trillion More</t>
-        </is>
-      </c>
-      <c r="G26" s="5" t="inlineStr">
-        <is>
-          <t>4,843,670,594,788</t>
-        </is>
-      </c>
+      <c r="A26" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>0xf3f83f6a5830e55b45b3c44010be0481baa1b9be</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>170,559,005,253,847</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="inlineStr">
+        <is>
+          <t>171 Trillion</t>
+        </is>
+      </c>
+      <c r="E26" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1706% </t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="n"/>
+      <c r="G26" s="2" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>0xf3f83f6a5830e55b45b3c44010be0481baa1b9be</t>
+          <t>0x4159fcaefd2216a1b581587ca97da9f53e8ba163</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>170,559,005,253,847</t>
+          <t>170,029,080,849,270</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t>171 Trillion</t>
+          <t>170 Trillion</t>
         </is>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1706% </t>
+          <t xml:space="preserve">0.1700% </t>
         </is>
       </c>
       <c r="F27" s="2" t="n"/>
@@ -1236,61 +1237,69 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>0x4159fcaefd2216a1b581587ca97da9f53e8ba163</t>
+          <t>0xbdf119001cf9d44d902bf7d8e283e10ab66ddeea</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>170,029,080,849,270</t>
+          <t>160,512,332,157,587</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>170 Trillion</t>
+          <t>161 Trillion</t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1700% </t>
+          <t xml:space="preserve">0.1605% </t>
         </is>
       </c>
       <c r="F28" s="2" t="n"/>
       <c r="G28" s="2" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>0xbdf119001cf9d44d902bf7d8e283e10ab66ddeea</t>
-        </is>
-      </c>
-      <c r="C29" s="3" t="inlineStr">
-        <is>
-          <t>160,512,332,157,587</t>
-        </is>
-      </c>
-      <c r="D29" s="3" t="inlineStr">
-        <is>
-          <t>161 Trillion</t>
-        </is>
-      </c>
-      <c r="E29" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1605% </t>
-        </is>
-      </c>
-      <c r="F29" s="2" t="n"/>
-      <c r="G29" s="2" t="n"/>
+      <c r="A29" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t>0xd693658b31ef059354118ac2b8067b989ebf4b2b</t>
+        </is>
+      </c>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>157,727,627,943,479</t>
+        </is>
+      </c>
+      <c r="D29" s="5" t="inlineStr">
+        <is>
+          <t>158 Trillion</t>
+        </is>
+      </c>
+      <c r="E29" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1577% </t>
+        </is>
+      </c>
+      <c r="F29" s="6" t="inlineStr">
+        <is>
+          <t>10 Trillion Less</t>
+        </is>
+      </c>
+      <c r="G29" s="7" t="inlineStr">
+        <is>
+          <t>9,607,900,318,418</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
@@ -1317,7 +1326,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
@@ -1344,7 +1353,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
@@ -1371,7 +1380,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
@@ -1398,7 +1407,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
@@ -1425,7 +1434,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
@@ -1452,7 +1461,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
@@ -1479,7 +1488,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
@@ -1506,7 +1515,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
@@ -1533,7 +1542,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
@@ -1560,7 +1569,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
@@ -1569,7 +1578,7 @@
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>109,231,111,388,513</t>
+          <t>109,294,002,133,176</t>
         </is>
       </c>
       <c r="D40" s="3" t="inlineStr">
@@ -1579,7 +1588,7 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1092% </t>
+          <t xml:space="preserve">0.1093% </t>
         </is>
       </c>
       <c r="F40" s="2" t="n"/>
@@ -1587,7 +1596,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
@@ -1614,7 +1623,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
@@ -1641,7 +1650,7 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
@@ -1668,7 +1677,7 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="4" t="inlineStr">
         <is>
@@ -1703,7 +1712,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
@@ -1730,7 +1739,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
@@ -1757,7 +1766,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
@@ -1784,7 +1793,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
@@ -1793,7 +1802,7 @@
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>100,372,973,911,978</t>
+          <t>100,429,972,530,650</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
@@ -1811,60 +1820,178 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>0x86437c0875fa78dc98c57bc010ef4ad07bc01715</t>
+          <t>0x302c44b648f5a84191f08551be26a2d2456a1fa1</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>100,127,887,461,980</t>
+          <t>93,336,673,893,067</t>
         </is>
       </c>
       <c r="D49" s="3" t="inlineStr">
         <is>
-          <t>100 Trillion</t>
+          <t>93 Trillion</t>
         </is>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1001% </t>
+          <t xml:space="preserve">0.0933% </t>
         </is>
       </c>
       <c r="F49" s="2" t="n"/>
       <c r="G49" s="2" t="n"/>
     </row>
+    <row r="51">
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t>Total's</t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="inlineStr">
+        <is>
+          <t>12,019,467,460,772,115</t>
+        </is>
+      </c>
+      <c r="D51" s="3" t="inlineStr">
+        <is>
+          <t>12019 Trillion</t>
+        </is>
+      </c>
+      <c r="E51" s="3" t="inlineStr">
+        <is>
+          <t>12.02%</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>-11 Trillion</t>
+        </is>
+      </c>
+      <c r="G51" s="2" t="inlineStr">
+        <is>
+          <t>-10,982,405,155,049</t>
+        </is>
+      </c>
+    </row>
     <row r="53">
-      <c r="B53" s="3" t="inlineStr">
-        <is>
-          <t>Total's</t>
-        </is>
-      </c>
-      <c r="C53" s="3" t="inlineStr">
-        <is>
-          <t>12,045,349,361,697,981</t>
-        </is>
-      </c>
-      <c r="D53" s="3" t="inlineStr">
-        <is>
-          <t>12045 Trillion</t>
-        </is>
-      </c>
-      <c r="E53" s="3" t="inlineStr">
-        <is>
-          <t>12.05%</t>
-        </is>
-      </c>
-      <c r="F53" s="2" t="inlineStr">
-        <is>
-          <t>9 Trillion</t>
-        </is>
-      </c>
-      <c r="G53" s="2" t="inlineStr">
-        <is>
-          <t>8,657,931,074,269</t>
+      <c r="A53" s="8" t="n"/>
+      <c r="B53" s="9" t="inlineStr">
+        <is>
+          <t>Old Whales</t>
+        </is>
+      </c>
+      <c r="C53" s="8" t="n"/>
+      <c r="D53" s="8" t="n"/>
+      <c r="E53" s="8" t="n"/>
+      <c r="F53" s="8" t="n"/>
+      <c r="G53" s="8" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B54" s="4" t="inlineStr">
+        <is>
+          <t>0x3d268cd580f89cfe6cc5dcf8764f51085f74a649</t>
+        </is>
+      </c>
+      <c r="C54" s="5" t="inlineStr">
+        <is>
+          <t>4,787,973,054,909</t>
+        </is>
+      </c>
+      <c r="D54" s="5" t="inlineStr">
+        <is>
+          <t>5 Trillion</t>
+        </is>
+      </c>
+      <c r="E54" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1278% </t>
+        </is>
+      </c>
+      <c r="F54" s="6" t="inlineStr">
+        <is>
+          <t>123 Trillion Less</t>
+        </is>
+      </c>
+      <c r="G54" s="7" t="inlineStr">
+        <is>
+          <t>123,043,494,726,928</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B55" s="4" t="inlineStr">
+        <is>
+          <t>0x505dd22c1bacced7531f319f5008318a440490bc</t>
+        </is>
+      </c>
+      <c r="C55" s="5" t="inlineStr">
+        <is>
+          <t>90,051,274,271,589</t>
+        </is>
+      </c>
+      <c r="D55" s="5" t="inlineStr">
+        <is>
+          <t>90 Trillion</t>
+        </is>
+      </c>
+      <c r="E55" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.0950% </t>
+        </is>
+      </c>
+      <c r="F55" s="6" t="inlineStr">
+        <is>
+          <t>5 Trillion Less</t>
+        </is>
+      </c>
+      <c r="G55" s="7" t="inlineStr">
+        <is>
+          <t>4,952,972,702,334</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B56" s="4" t="inlineStr">
+        <is>
+          <t>0x2bd6997bf6fcfde139eb1b9346fbf79defd4e8cc</t>
+        </is>
+      </c>
+      <c r="C56" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D56" s="5" t="inlineStr">
+        <is>
+          <t>0 Trillion</t>
+        </is>
+      </c>
+      <c r="E56" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.5497% </t>
+        </is>
+      </c>
+      <c r="F56" s="6" t="inlineStr">
+        <is>
+          <t>550 Trillion Less</t>
+        </is>
+      </c>
+      <c r="G56" s="7" t="inlineStr">
+        <is>
+          <t>549,662,717,019,826</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add full total gain / loss
</commit_message>
<xml_diff>
--- a/WhaleWatching/holders.xlsx
+++ b/WhaleWatching/holders.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,7 +503,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
@@ -530,7 +530,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
@@ -557,7 +557,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
@@ -584,7 +584,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
@@ -611,7 +611,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
@@ -646,7 +646,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
@@ -727,7 +727,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
@@ -754,7 +754,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
@@ -781,7 +781,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
@@ -808,7 +808,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
@@ -835,7 +835,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
@@ -862,7 +862,7 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
@@ -897,7 +897,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
@@ -924,7 +924,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
@@ -951,7 +951,7 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
@@ -986,7 +986,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
@@ -1156,7 +1156,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
@@ -1210,7 +1210,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="29">
       <c r="A29" s="4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="4" t="inlineStr">
         <is>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
@@ -1848,7 +1848,7 @@
     <row r="51">
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>Total's</t>
+          <t>Total's for top 50 (actually 48)</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
@@ -1892,106 +1892,124 @@
     </row>
     <row r="54">
       <c r="A54" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>0x3d268cd580f89cfe6cc5dcf8764f51085f74a649</t>
+          <t>0x2bd6997bf6fcfde139eb1b9346fbf79defd4e8cc</t>
         </is>
       </c>
       <c r="C54" s="5" t="inlineStr">
         <is>
-          <t>4,787,973,054,909</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D54" s="5" t="inlineStr">
         <is>
-          <t>5 Trillion</t>
+          <t>0 Trillion</t>
         </is>
       </c>
       <c r="E54" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1278% </t>
+          <t xml:space="preserve">0.5497% </t>
         </is>
       </c>
       <c r="F54" s="6" t="inlineStr">
         <is>
-          <t>123 Trillion Less</t>
+          <t>550 Trillion Less</t>
         </is>
       </c>
       <c r="G54" s="7" t="inlineStr">
         <is>
-          <t>123,043,494,726,928</t>
+          <t>549,662,717,019,826</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>0x505dd22c1bacced7531f319f5008318a440490bc</t>
+          <t>0x3d268cd580f89cfe6cc5dcf8764f51085f74a649</t>
         </is>
       </c>
       <c r="C55" s="5" t="inlineStr">
         <is>
-          <t>90,051,274,271,589</t>
+          <t>4,787,982,343,926</t>
         </is>
       </c>
       <c r="D55" s="5" t="inlineStr">
         <is>
-          <t>90 Trillion</t>
+          <t>5 Trillion</t>
         </is>
       </c>
       <c r="E55" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0950% </t>
+          <t xml:space="preserve">0.1278% </t>
         </is>
       </c>
       <c r="F55" s="6" t="inlineStr">
         <is>
-          <t>5 Trillion Less</t>
+          <t>123 Trillion Less</t>
         </is>
       </c>
       <c r="G55" s="7" t="inlineStr">
         <is>
-          <t>4,952,972,702,334</t>
+          <t>123,043,485,437,911</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>0x2bd6997bf6fcfde139eb1b9346fbf79defd4e8cc</t>
+          <t>0x505dd22c1bacced7531f319f5008318a440490bc</t>
         </is>
       </c>
       <c r="C56" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>90,051,450,064,196</t>
         </is>
       </c>
       <c r="D56" s="5" t="inlineStr">
         <is>
-          <t>0 Trillion</t>
+          <t>90 Trillion</t>
         </is>
       </c>
       <c r="E56" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.5497% </t>
+          <t xml:space="preserve">0.0950% </t>
         </is>
       </c>
       <c r="F56" s="6" t="inlineStr">
         <is>
-          <t>550 Trillion Less</t>
+          <t>5 Trillion Less</t>
         </is>
       </c>
       <c r="G56" s="7" t="inlineStr">
         <is>
-          <t>549,662,717,019,826</t>
+          <t>4,952,796,909,727</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="D58" s="6" t="n"/>
+      <c r="E58" s="7" t="inlineStr">
+        <is>
+          <t>Total loss / gain from all whales</t>
+        </is>
+      </c>
+      <c r="F58" s="6" t="inlineStr">
+        <is>
+          <t>-689 Trillion</t>
+        </is>
+      </c>
+      <c r="G58" s="6" t="inlineStr">
+        <is>
+          <t>-688,641,404,522,513</t>
         </is>
       </c>
     </row>

</xml_diff>